<commit_message>
Iniciando automatização de testes
</commit_message>
<xml_diff>
--- a/PlanoDeTestes/ParaBank.xlsx
+++ b/PlanoDeTestes/ParaBank.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130C7007-4AF8-4544-8590-ED532D7FA7C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF203A0-26D0-4936-AE4A-BCC016238470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sumário" sheetId="1" r:id="rId1"/>
@@ -819,7 +819,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3"/>
+        <fgColor theme="1" tint="4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1149,27 +1149,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1188,28 +1167,43 @@
     <xf numFmtId="10" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1220,17 +1214,23 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1763,8 +1763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1781,78 +1781,78 @@
   <sheetData>
     <row r="1" spans="1:7" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="32"/>
-      <c r="G2" s="33"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="31"/>
     </row>
     <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="27" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="34" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="27" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="22"/>
+      <c r="E4" s="13"/>
       <c r="F4" s="6"/>
-      <c r="G4" s="23"/>
+      <c r="G4" s="14"/>
     </row>
     <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="27" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="22"/>
+      <c r="E5" s="13"/>
       <c r="F5" s="6"/>
-      <c r="G5" s="23"/>
+      <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="37">
+      <c r="B6" s="19">
         <v>45175</v>
       </c>
-      <c r="E6" s="22"/>
+      <c r="E6" s="13"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="23"/>
+      <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="28" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="24"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="26"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1871,8 +1871,8 @@
   </sheetPr>
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1887,931 +1887,931 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="25" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="F2" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="28"/>
+      <c r="F2" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="18"/>
     </row>
     <row r="3" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="F3" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="28"/>
+      <c r="F3" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="18"/>
     </row>
     <row r="4" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="F4" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="28"/>
+      <c r="F4" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="18"/>
     </row>
     <row r="5" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="F5" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="28"/>
+      <c r="F5" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="18"/>
     </row>
     <row r="6" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="F6" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="28"/>
+      <c r="F6" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="18"/>
     </row>
     <row r="7" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F7" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="28"/>
+      <c r="F7" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="18"/>
     </row>
     <row r="8" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="28"/>
+      <c r="F8" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="18"/>
     </row>
     <row r="9" spans="1:7" ht="244.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="F9" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="28"/>
+      <c r="F9" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="18"/>
     </row>
     <row r="10" spans="1:7" ht="230.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="28" t="s">
+      <c r="G10" s="18" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="230.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="E11" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="F11" s="28" t="s">
+      <c r="F11" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="28" t="s">
+      <c r="G11" s="18" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="244.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="28" t="s">
+      <c r="E12" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="F12" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="28"/>
+      <c r="F12" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="18"/>
     </row>
     <row r="13" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="E13" s="28" t="s">
+      <c r="E13" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="F13" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" s="28"/>
+      <c r="F13" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="18"/>
     </row>
     <row r="14" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E14" s="28" t="s">
+      <c r="E14" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="F14" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G14" s="28"/>
+      <c r="F14" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="28" t="s">
+      <c r="D15" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="E15" s="28" t="s">
+      <c r="E15" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="F15" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G15" s="28"/>
+      <c r="F15" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="D16" s="28" t="s">
+      <c r="D16" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E16" s="28" t="s">
+      <c r="E16" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="F16" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G16" s="28"/>
+      <c r="F16" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="E17" s="28" t="s">
+      <c r="E17" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="F17" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G17" s="28"/>
+      <c r="F17" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="28" t="s">
+      <c r="C18" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="D18" s="28" t="s">
+      <c r="D18" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="E18" s="28" t="s">
+      <c r="E18" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="F18" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G18" s="28"/>
+      <c r="F18" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="D19" s="28" t="s">
+      <c r="D19" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="E19" s="28" t="s">
+      <c r="E19" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="F19" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G19" s="28"/>
+      <c r="F19" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="C20" s="28" t="s">
+      <c r="C20" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="D20" s="28" t="s">
+      <c r="D20" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="E20" s="28" t="s">
+      <c r="E20" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="F20" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G20" s="28"/>
+      <c r="F20" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="C21" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="D21" s="28" t="s">
+      <c r="D21" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="E21" s="28" t="s">
+      <c r="E21" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="F21" s="28" t="s">
+      <c r="F21" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="G21" s="28" t="s">
+      <c r="G21" s="18" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="28" t="s">
+      <c r="A22" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="D22" s="28" t="s">
+      <c r="D22" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="E22" s="28" t="s">
+      <c r="E22" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="F22" s="28" t="s">
+      <c r="F22" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="G22" s="28" t="s">
+      <c r="G22" s="18" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="28" t="e">
-        <f t="shared" ref="A23:A24" si="0">A22+1</f>
+      <c r="A23" s="18" t="e">
+        <f t="shared" ref="A23" si="0">A22+1</f>
         <v>#VALUE!</v>
       </c>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28" t="s">
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="G23" s="28"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="28" t="s">
+      <c r="A24" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="B24" s="28" t="s">
+      <c r="B24" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="28" t="s">
+      <c r="C24" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="D24" s="28" t="s">
+      <c r="D24" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="E24" s="28" t="s">
+      <c r="E24" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="F24" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G24" s="28"/>
+      <c r="F24" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="28" t="s">
+      <c r="A25" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C25" s="28" t="s">
+      <c r="C25" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="D25" s="28" t="s">
+      <c r="D25" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="E25" s="28" t="s">
+      <c r="E25" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="F25" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G25" s="28"/>
+      <c r="F25" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C26" s="28" t="s">
+      <c r="C26" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="D26" s="28" t="s">
+      <c r="D26" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="E26" s="28" t="s">
+      <c r="E26" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="F26" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G26" s="28"/>
+      <c r="F26" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C27" s="28" t="s">
+      <c r="C27" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="D27" s="28" t="s">
+      <c r="D27" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="E27" s="28" t="s">
+      <c r="E27" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="F27" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G27" s="28"/>
+      <c r="F27" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="B28" s="28" t="s">
+      <c r="B28" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C28" s="28" t="s">
+      <c r="C28" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="D28" s="28" t="s">
+      <c r="D28" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="E28" s="28" t="s">
+      <c r="E28" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="F28" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G28" s="28"/>
+      <c r="F28" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="28" t="s">
+      <c r="A29" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C29" s="28" t="s">
+      <c r="C29" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="D29" s="28" t="s">
+      <c r="D29" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="E29" s="28" t="s">
+      <c r="E29" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="F29" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G29" s="28"/>
+      <c r="F29" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G29" s="18"/>
     </row>
     <row r="30" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="28" t="s">
+      <c r="A30" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="B30" s="28" t="s">
+      <c r="B30" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C30" s="28" t="s">
+      <c r="C30" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="D30" s="28" t="s">
+      <c r="D30" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="E30" s="28" t="s">
+      <c r="E30" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="F30" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G30" s="28"/>
+      <c r="F30" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="28" t="s">
+      <c r="A31" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="B31" s="28" t="s">
+      <c r="B31" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C31" s="28" t="s">
+      <c r="C31" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="D31" s="28" t="s">
+      <c r="D31" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="F31" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G31" s="28"/>
+      <c r="F31" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G31" s="18"/>
     </row>
     <row r="32" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="28" t="s">
+      <c r="A32" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="B32" s="28" t="s">
+      <c r="B32" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C32" s="28" t="s">
+      <c r="C32" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="D32" s="28" t="s">
+      <c r="D32" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="E32" s="28" t="s">
+      <c r="E32" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="F32" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G32" s="28"/>
+      <c r="F32" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="28" t="s">
+      <c r="A33" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="B33" s="28" t="s">
+      <c r="B33" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C33" s="28" t="s">
+      <c r="C33" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="D33" s="28" t="s">
+      <c r="D33" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="E33" s="28" t="s">
+      <c r="E33" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="F33" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G33" s="28"/>
+      <c r="F33" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="28" t="s">
+      <c r="A34" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="B34" s="28" t="s">
+      <c r="B34" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C34" s="28" t="s">
+      <c r="C34" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="D34" s="28" t="s">
+      <c r="D34" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="E34" s="28" t="s">
+      <c r="E34" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="F34" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G34" s="28"/>
+      <c r="F34" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A35" s="28" t="s">
+      <c r="A35" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="B35" s="28" t="s">
+      <c r="B35" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C35" s="28" t="s">
+      <c r="C35" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="D35" s="28" t="s">
+      <c r="D35" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="E35" s="28" t="s">
+      <c r="E35" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="F35" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G35" s="28"/>
+      <c r="F35" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A36" s="28" t="s">
+      <c r="A36" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="B36" s="28" t="s">
+      <c r="B36" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C36" s="28" t="s">
+      <c r="C36" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="D36" s="28" t="s">
+      <c r="D36" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="E36" s="28" t="s">
+      <c r="E36" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="F36" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G36" s="28"/>
+      <c r="F36" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A37" s="28" t="s">
+      <c r="A37" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="B37" s="28" t="s">
+      <c r="B37" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C37" s="28" t="s">
+      <c r="C37" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="D37" s="28" t="s">
+      <c r="D37" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="E37" s="28" t="s">
+      <c r="E37" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="F37" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G37" s="28"/>
+      <c r="F37" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="28" t="s">
+      <c r="A38" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="B38" s="28" t="s">
+      <c r="B38" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C38" s="28" t="s">
+      <c r="C38" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="D38" s="28" t="s">
+      <c r="D38" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="E38" s="28" t="s">
+      <c r="E38" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="F38" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G38" s="28"/>
+      <c r="F38" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G38" s="18"/>
     </row>
     <row r="39" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="28" t="s">
+      <c r="A39" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="B39" s="28" t="s">
+      <c r="B39" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C39" s="28" t="s">
+      <c r="C39" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="D39" s="28" t="s">
+      <c r="D39" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="E39" s="28" t="s">
+      <c r="E39" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="F39" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G39" s="28"/>
+      <c r="F39" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G39" s="18"/>
     </row>
     <row r="40" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A40" s="28" t="s">
+      <c r="A40" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="B40" s="28" t="s">
+      <c r="B40" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C40" s="28" t="s">
+      <c r="C40" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="D40" s="28" t="s">
+      <c r="D40" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="E40" s="28" t="s">
+      <c r="E40" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="F40" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G40" s="28"/>
+      <c r="F40" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G40" s="18"/>
     </row>
     <row r="41" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A41" s="28" t="s">
+      <c r="A41" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="B41" s="28" t="s">
+      <c r="B41" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C41" s="28" t="s">
+      <c r="C41" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="D41" s="28" t="s">
+      <c r="D41" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="E41" s="28" t="s">
+      <c r="E41" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="F41" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G41" s="28"/>
+      <c r="F41" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G41" s="18"/>
     </row>
     <row r="42" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A42" s="28" t="s">
+      <c r="A42" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="B42" s="28" t="s">
+      <c r="B42" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C42" s="28" t="s">
+      <c r="C42" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="D42" s="28" t="s">
+      <c r="D42" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="E42" s="28" t="s">
+      <c r="E42" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="F42" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G42" s="28"/>
+      <c r="F42" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G42" s="18"/>
     </row>
     <row r="43" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A43" s="28" t="s">
+      <c r="A43" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="B43" s="28" t="s">
+      <c r="B43" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C43" s="28" t="s">
+      <c r="C43" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="D43" s="28" t="s">
+      <c r="D43" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="E43" s="28" t="s">
+      <c r="E43" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="F43" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G43" s="28"/>
+      <c r="F43" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G43" s="18"/>
     </row>
     <row r="44" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A44" s="28" t="s">
+      <c r="A44" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="B44" s="28" t="s">
+      <c r="B44" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C44" s="28" t="s">
+      <c r="C44" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="D44" s="28" t="s">
+      <c r="D44" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="E44" s="28" t="s">
+      <c r="E44" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="F44" s="28" t="s">
+      <c r="F44" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="G44" s="28" t="s">
+      <c r="G44" s="18" t="s">
         <v>143</v>
       </c>
     </row>
@@ -2842,7 +2842,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2854,59 +2854,59 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:3" ht="26.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="36"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="22"/>
     </row>
     <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="7">
         <f>COUNTA(Cenários!B:B)-1</f>
         <v>42</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="8">
         <f>COUNTIF(Cenários!F:F,"OK")</f>
         <v>37</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="11">
         <f>B4/B3</f>
         <v>0.88095238095238093</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="8">
         <f>COUNTIF(Cenários!F:F,"NOK")</f>
         <v>5</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="11">
         <f>B5/B3</f>
         <v>0.11904761904761904</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="16">
+      <c r="B6" s="9">
         <f>B3-B4-B5</f>
         <v>0</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="12">
         <f>B6/B3</f>
         <v>0</v>
       </c>

</xml_diff>